<commit_message>
added SoGou and basic start to Calc. Diffs.
</commit_message>
<xml_diff>
--- a/Source [TEST].xlsx
+++ b/Source [TEST].xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfitz\Google Drive\Docs\VSCode\Work\Translating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfitz\Documents\GitHub Clones\machine-translation-scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B606A162-DA21-482A-BF99-3E2BBA5610B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D609611-7AA1-4EF0-A6C1-454DC0B82399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="4005" windowWidth="14955" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="1080" windowWidth="14955" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>你的呼吸道感染是由冠状病毒引起的。  </t>
   </si>
@@ -264,10 +264,10 @@
     <t>Project</t>
   </si>
   <si>
-    <t>한국어</t>
-  </si>
-  <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>中文</t>
   </si>
 </sst>
 </file>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,10 +607,10 @@
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>IF($B$1="한국어", 'KO test'!A1, IF($B$1="中文", 'ZH test'!A1, 'JP test'!A7))</f>
-        <v>포포, 이리 오너라!</v>
+        <v>你的呼吸道感染是由冠状病毒引起的。  </v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>76</v>
@@ -619,10 +619,10 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF($B$1="한국어", 'KO test'!A2, IF($B$1="中文", 'ZH test'!A2, 'JP test'!A8))</f>
-        <v>앗! 저 도깨비 녀석!</v>
+        <v>犬冠状病毒病。</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -631,265 +631,193 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF($B$1="한국어", 'KO test'!A3, IF($B$1="中文", 'ZH test'!A3, 'JP test'!A9))</f>
-        <v>음? 이 아이를 아는가?</v>
+        <v>新生犊腹泻冠状病毒。</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF($B$1="한국어", 'KO test'!A4, IF($B$1="中文", 'ZH test'!A4, 'JP test'!A10))</f>
-        <v>저 녀석이 우리를 이곳으로 끌고 왔다고!</v>
+        <v>猪传染性胃肠炎冠状病毒。  </v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF($B$1="한국어", 'KO test'!A5, IF($B$1="中文", 'ZH test'!A5, 'JP test'!A11))</f>
-        <v>기껏 도와줬더니!</v>
+        <v>大熊猫犬冠状病毒的分离与鉴定。  </v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF($B$1="한국어", 'KO test'!A6, IF($B$1="中文", 'ZH test'!A6, 'JP test'!A12))</f>
-        <v>그 전에 그쪽이 먼저 불덩어리를 던지지 않았슙니까?!</v>
+        <v>冠状病毒感染引起水貂肠炎的诊断。 </v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF($B$1="한국어", 'KO test'!A7, IF($B$1="中文", 'ZH test'!A7, 'JP test'!A13))</f>
-        <v>그리고 끌고 간 적 없슙니다!</v>
+        <v>禽冠状病毒的介电松弛效应及灭活。  </v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF($B$1="한국어", 'KO test'!A8, IF($B$1="中文", 'ZH test'!A8, 'JP test'!A14))</f>
-        <v>그쪽이 멋대로 따라온 겁니다!</v>
+        <v>冠状病毒基因组发明专利保护的思考。  </v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF($B$1="한국어", 'KO test'!A9, IF($B$1="中文", 'ZH test'!A9, 'JP test'!A15))</f>
-        <v>따라간 건 아닌데….</v>
+        <v>中和试验进一步证明该分离病毒是一种犬冠状病毒。  </v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF($B$1="한국어", 'KO test'!A10, IF($B$1="中文", 'ZH test'!A10, 'JP test'!A16))</f>
-        <v>그래서 몬스터들한테 두들겨 맞고 있는 걸 구해준 게 누군데?!</v>
+        <v>基于密码子使用模式的冠状病毒亲缘关系分析。  </v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF($B$1="한국어", 'KO test'!A11, IF($B$1="中文", 'ZH test'!A11, 'JP test'!A17))</f>
-        <v>윽… 그…그건….</v>
+        <v>猪呼吸道冠状病毒及实验室诊断方法研究进展。  </v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF($B$1="한국어", 'KO test'!A12, IF($B$1="中文", 'ZH test'!A12, 'JP test'!A18))</f>
-        <v>그러니까 주기로 한 건 주고 가야지!</v>
+        <v>与犬细小病毒，但没有具体的治疗犬冠状病毒。  </v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF($B$1="한국어", 'KO test'!A13, IF($B$1="中文", 'ZH test'!A13, 'JP test'!A19))</f>
-        <v>준다 한 적 없슙니다!</v>
+        <v>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。  </v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF($B$1="한국어", 'KO test'!A14, IF($B$1="中文", 'ZH test'!A14, 'JP test'!A20))</f>
-        <v>지금 떼어먹겠다는 거야?!</v>
+        <v>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。 </v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF($B$1="한국어", 'KO test'!A15, IF($B$1="中文", 'ZH test'!A15, 'JP test'!A21))</f>
-        <v>흐음... 그렇게 된 게로군.</v>
+        <v>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。  </v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF($B$1="한국어", 'KO test'!A16, IF($B$1="中文", 'ZH test'!A16, 'JP test'!A22))</f>
-        <v>이 녀석, 또 땡땡이 치고 나가더니 이런 사고를….</v>
+        <v>病毒被反病毒软件删除了。  </v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF($B$1="한국어", 'KO test'!A17, IF($B$1="中文", 'ZH test'!A17, 'JP test'!A23))</f>
-        <v>죄… 죄숑합니다….</v>
+        <v>他染上了一种致命病毒。  </v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF($B$1="한국어", 'KO test'!A18, IF($B$1="中文", 'ZH test'!A18, 'JP test'!A24))</f>
-        <v>그래도 회니르 님이 일으키시는 사고에 비하면 약과네요.</v>
+        <v>血液检验显示有病毒存在。  </v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF($B$1="한국어", 'KO test'!A19, IF($B$1="中文", 'ZH test'!A19, 'JP test'!A25))</f>
-        <v>그건 맞슙니다!</v>
+        <v>哎呀，电脑又有病毒了。  </v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF($B$1="한국어", 'KO test'!A20, IF($B$1="中文", 'ZH test'!A20, 'JP test'!A26))</f>
-        <v>내… 내가 언제 사고를 쳤다고 그러나?</v>
+        <v>你的呼吸道感染是由冠状病毒引起的。  </v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF($B$1="한국어", 'KO test'!A21, IF($B$1="中文", 'ZH test'!A21, 'JP test'!A27))</f>
-        <v>저번에 뭔가를 찾는다고 차원을 온통 휘젓지 않으셨나요?</v>
+        <v>犬冠状病毒病。</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF($B$1="한국어", 'KO test'!A26, IF($B$1="中文", 'ZH test'!A26, 'JP test'!A32))</f>
-        <v>어쨌든 우리 포포가 신세를 진 것 같군.</v>
+        <v>禽冠状病毒的介电松弛效应及灭活。  </v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF($B$1="한국어", 'KO test'!A27, IF($B$1="中文", 'ZH test'!A27, 'JP test'!A33))</f>
-        <v>내 적당히 자네들에게 줄 만한 물건을 찾아보도록 하지.</v>
+        <v>冠状病毒基因组发明专利保护的思考。  </v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF($B$1="한국어", 'KO test'!A28, IF($B$1="中文", 'ZH test'!A28, 'JP test'!A34))</f>
-        <v>다행이네요, 리나 씨.</v>
+        <v>中和试验进一步证明该分离病毒是一种犬冠状病毒。  </v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF($B$1="한국어", 'KO test'!A29, IF($B$1="中文", 'ZH test'!A29, 'JP test'!A35))</f>
-        <v>다행은 무슨!</v>
+        <v>基于密码子使用模式的冠状病毒亲缘关系分析。  </v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF($B$1="한국어", 'KO test'!A30, IF($B$1="中文", 'ZH test'!A30, 'JP test'!A36))</f>
-        <v>원래 받아야 하는 거잖아?</v>
+        <v>猪呼吸道冠状病毒及实验室诊断方法研究进展。  </v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF($B$1="한국어", 'KO test'!A31, IF($B$1="中文", 'ZH test'!A31, 'JP test'!A37))</f>
-        <v>이런 걸 떼먹히면 이 리나 워드도티르 님의 이름이 운다고!</v>
+        <v>与犬细小病毒，但没有具体的治疗犬冠状病毒。  </v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF($B$1="한국어", 'KO test'!A32, IF($B$1="中文", 'ZH test'!A32, 'JP test'!A38))</f>
-        <v>자네, 이름이 뭐라고 했는가?</v>
+        <v>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。  </v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF($B$1="한국어", 'KO test'!A33, IF($B$1="中文", 'ZH test'!A33, 'JP test'!A39))</f>
-        <v>내 이름?</v>
+        <v>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。 </v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF($B$1="한국어", 'KO test'!A34, IF($B$1="中文", 'ZH test'!A34, 'JP test'!A40))</f>
-        <v>리나.</v>
+        <v>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。  </v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF($B$1="한국어", 'KO test'!A35, IF($B$1="中文", 'ZH test'!A35, 'JP test'!A41))</f>
-        <v>아니, 풀네임이 뭐라고?</v>
+        <v>病毒被反病毒软件删除了。  </v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF($B$1="한국어", 'KO test'!A36, IF($B$1="中文", 'ZH test'!A36, 'JP test'!A42))</f>
-        <v>리나 워드도티르인데.</v>
+        <v>他染上了一种致命病毒。  </v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF($B$1="한국어", 'KO test'!A37, IF($B$1="中文", 'ZH test'!A37, 'JP test'!A43))</f>
-        <v>리나… 워드도티르라면….</v>
+        <v>血液检验显示有病毒存在。  </v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" t="str">
         <f>IF($B$1="한국어", 'KO test'!A38, IF($B$1="中文", 'ZH test'!A38, 'JP test'!A44))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f>IF($B$1="한국어", 'KO test'!A39, IF($B$1="中文", 'ZH test'!A39, 'JP test'!A45))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f>IF($B$1="한국어", 'KO test'!A40, IF($B$1="中文", 'ZH test'!A40, 'JP test'!A46))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f>IF($B$1="한국어", 'KO test'!A41, IF($B$1="中文", 'ZH test'!A41, 'JP test'!A47))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f>IF($B$1="한국어", 'KO test'!A42, IF($B$1="中文", 'ZH test'!A42, 'JP test'!A48))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <f>IF($B$1="한국어", 'KO test'!A43, IF($B$1="中文", 'ZH test'!A43, 'JP test'!A49))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <f>IF($B$1="한국어", 'KO test'!A44, IF($B$1="中文", 'ZH test'!A44, 'JP test'!A50))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f>IF($B$1="한국어", 'KO test'!A45, IF($B$1="中文", 'ZH test'!A45, 'JP test'!A51))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <f>IF($B$1="한국어", 'KO test'!A46, IF($B$1="中文", 'ZH test'!A46, 'JP test'!A52))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <f>IF($B$1="한국어", 'KO test'!A47, IF($B$1="中文", 'ZH test'!A47, 'JP test'!A53))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <f>IF($B$1="한국어", 'KO test'!A48, IF($B$1="中文", 'ZH test'!A48, 'JP test'!A54))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f>IF($B$1="한국어", 'KO test'!A49, IF($B$1="中文", 'ZH test'!A49, 'JP test'!A55))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f>IF($B$1="한국어", 'KO test'!A50, IF($B$1="中文", 'ZH test'!A50, 'JP test'!A56))</f>
-        <v>0</v>
+        <v>哎呀，电脑又有病毒了。  </v>
       </c>
     </row>
   </sheetData>
@@ -1219,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D58F233-F40F-4825-BB23-37CF2E70714B}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection sqref="A1:A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,6 +1250,101 @@
         <v>18</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed DeepL and started function-ifying
</commit_message>
<xml_diff>
--- a/Source [TEST].xlsx
+++ b/Source [TEST].xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfitz\Documents\GitHub Clones\machine-translation-scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Documents\GitHub Clones\machine-translation-scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D609611-7AA1-4EF0-A6C1-454DC0B82399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353335BA-A23B-41E4-A2FE-27324CF555AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="1080" windowWidth="14955" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17625" yWindow="13575" windowWidth="23595" windowHeight="16110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -30,63 +30,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
-    <t>你的呼吸道感染是由冠状病毒引起的。  </t>
-  </si>
-  <si>
     <t>犬冠状病毒病。</t>
   </si>
   <si>
     <t>新生犊腹泻冠状病毒。</t>
   </si>
   <si>
-    <t>猪传染性胃肠炎冠状病毒。  </t>
-  </si>
-  <si>
-    <t>大熊猫犬冠状病毒的分离与鉴定。  </t>
-  </si>
-  <si>
-    <t>冠状病毒感染引起水貂肠炎的诊断。 </t>
-  </si>
-  <si>
-    <t>禽冠状病毒的介电松弛效应及灭活。  </t>
-  </si>
-  <si>
-    <t>冠状病毒基因组发明专利保护的思考。  </t>
-  </si>
-  <si>
-    <t>中和试验进一步证明该分离病毒是一种犬冠状病毒。  </t>
-  </si>
-  <si>
-    <t>基于密码子使用模式的冠状病毒亲缘关系分析。  </t>
-  </si>
-  <si>
-    <t>猪呼吸道冠状病毒及实验室诊断方法研究进展。  </t>
-  </si>
-  <si>
-    <t>与犬细小病毒，但没有具体的治疗犬冠状病毒。  </t>
-  </si>
-  <si>
-    <t>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。  </t>
-  </si>
-  <si>
-    <t>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。 </t>
-  </si>
-  <si>
-    <t>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。  </t>
-  </si>
-  <si>
-    <t>病毒被反病毒软件删除了。  </t>
-  </si>
-  <si>
-    <t>他染上了一种致命病毒。  </t>
-  </si>
-  <si>
-    <t>血液检验显示有病毒存在。  </t>
-  </si>
-  <si>
-    <t>哎呀，电脑又有病毒了。  </t>
-  </si>
-  <si>
     <t>포포, 이리 오너라!</t>
   </si>
   <si>
@@ -268,6 +217,57 @@
   </si>
   <si>
     <t>中文</t>
+  </si>
+  <si>
+    <t>你的呼吸道感染是由冠状病毒引起的。</t>
+  </si>
+  <si>
+    <t>猪传染性胃肠炎冠状病毒。</t>
+  </si>
+  <si>
+    <t>大熊猫犬冠状病毒的分离与鉴定。</t>
+  </si>
+  <si>
+    <t>冠状病毒感染引起水貂肠炎的诊断。</t>
+  </si>
+  <si>
+    <t>禽冠状病毒的介电松弛效应及灭活。</t>
+  </si>
+  <si>
+    <t>冠状病毒基因组发明专利保护的思考。</t>
+  </si>
+  <si>
+    <t>中和试验进一步证明该分离病毒是一种犬冠状病毒。</t>
+  </si>
+  <si>
+    <t>基于密码子使用模式的冠状病毒亲缘关系分析。</t>
+  </si>
+  <si>
+    <t>猪呼吸道冠状病毒及实验室诊断方法研究进展。</t>
+  </si>
+  <si>
+    <t>与犬细小病毒，但没有具体的治疗犬冠状病毒。</t>
+  </si>
+  <si>
+    <t>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。</t>
+  </si>
+  <si>
+    <t>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。</t>
+  </si>
+  <si>
+    <t>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。</t>
+  </si>
+  <si>
+    <t>病毒被反病毒软件删除了。</t>
+  </si>
+  <si>
+    <t>他染上了一种致命病毒。</t>
+  </si>
+  <si>
+    <t>血液检验显示有病毒存在。</t>
+  </si>
+  <si>
+    <t>哎呀，电脑又有病毒了。</t>
   </si>
 </sst>
 </file>
@@ -594,9 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A47"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -607,13 +605,13 @@
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>IF($B$1="한국어", 'KO test'!A1, IF($B$1="中文", 'ZH test'!A1, 'JP test'!A7))</f>
-        <v>你的呼吸道感染是由冠状病毒引起的。  </v>
+        <v>你的呼吸道感染是由冠状病毒引起的。</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,10 +620,10 @@
         <v>犬冠状病毒病。</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,103 +635,103 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF($B$1="한국어", 'KO test'!A4, IF($B$1="中文", 'ZH test'!A4, 'JP test'!A10))</f>
-        <v>猪传染性胃肠炎冠状病毒。  </v>
+        <v>猪传染性胃肠炎冠状病毒。</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF($B$1="한국어", 'KO test'!A5, IF($B$1="中文", 'ZH test'!A5, 'JP test'!A11))</f>
-        <v>大熊猫犬冠状病毒的分离与鉴定。  </v>
+        <v>大熊猫犬冠状病毒的分离与鉴定。</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF($B$1="한국어", 'KO test'!A6, IF($B$1="中文", 'ZH test'!A6, 'JP test'!A12))</f>
-        <v>冠状病毒感染引起水貂肠炎的诊断。 </v>
+        <v>冠状病毒感染引起水貂肠炎的诊断。</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF($B$1="한국어", 'KO test'!A7, IF($B$1="中文", 'ZH test'!A7, 'JP test'!A13))</f>
-        <v>禽冠状病毒的介电松弛效应及灭活。  </v>
+        <v>禽冠状病毒的介电松弛效应及灭活。</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF($B$1="한국어", 'KO test'!A8, IF($B$1="中文", 'ZH test'!A8, 'JP test'!A14))</f>
-        <v>冠状病毒基因组发明专利保护的思考。  </v>
+        <v>冠状病毒基因组发明专利保护的思考。</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF($B$1="한국어", 'KO test'!A9, IF($B$1="中文", 'ZH test'!A9, 'JP test'!A15))</f>
-        <v>中和试验进一步证明该分离病毒是一种犬冠状病毒。  </v>
+        <v>中和试验进一步证明该分离病毒是一种犬冠状病毒。</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF($B$1="한국어", 'KO test'!A10, IF($B$1="中文", 'ZH test'!A10, 'JP test'!A16))</f>
-        <v>基于密码子使用模式的冠状病毒亲缘关系分析。  </v>
+        <v>基于密码子使用模式的冠状病毒亲缘关系分析。</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF($B$1="한국어", 'KO test'!A11, IF($B$1="中文", 'ZH test'!A11, 'JP test'!A17))</f>
-        <v>猪呼吸道冠状病毒及实验室诊断方法研究进展。  </v>
+        <v>猪呼吸道冠状病毒及实验室诊断方法研究进展。</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF($B$1="한국어", 'KO test'!A12, IF($B$1="中文", 'ZH test'!A12, 'JP test'!A18))</f>
-        <v>与犬细小病毒，但没有具体的治疗犬冠状病毒。  </v>
+        <v>与犬细小病毒，但没有具体的治疗犬冠状病毒。</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF($B$1="한국어", 'KO test'!A13, IF($B$1="中文", 'ZH test'!A13, 'JP test'!A19))</f>
-        <v>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。  </v>
+        <v>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF($B$1="한국어", 'KO test'!A14, IF($B$1="中文", 'ZH test'!A14, 'JP test'!A20))</f>
-        <v>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。 </v>
+        <v>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF($B$1="한국어", 'KO test'!A15, IF($B$1="中文", 'ZH test'!A15, 'JP test'!A21))</f>
-        <v>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。  </v>
+        <v>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF($B$1="한국어", 'KO test'!A16, IF($B$1="中文", 'ZH test'!A16, 'JP test'!A22))</f>
-        <v>病毒被反病毒软件删除了。  </v>
+        <v>病毒被反病毒软件删除了。</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF($B$1="한국어", 'KO test'!A17, IF($B$1="中文", 'ZH test'!A17, 'JP test'!A23))</f>
-        <v>他染上了一种致命病毒。  </v>
+        <v>他染上了一种致命病毒。</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF($B$1="한국어", 'KO test'!A18, IF($B$1="中文", 'ZH test'!A18, 'JP test'!A24))</f>
-        <v>血液检验显示有病毒存在。  </v>
+        <v>血液检验显示有病毒存在。</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF($B$1="한국어", 'KO test'!A19, IF($B$1="中文", 'ZH test'!A19, 'JP test'!A25))</f>
-        <v>哎呀，电脑又有病毒了。  </v>
+        <v>哎呀，电脑又有病毒了。</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF($B$1="한국어", 'KO test'!A20, IF($B$1="中文", 'ZH test'!A20, 'JP test'!A26))</f>
-        <v>你的呼吸道感染是由冠状病毒引起的。  </v>
+        <v>你的呼吸道感染是由冠状病毒引起的。</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -745,79 +743,79 @@
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF($B$1="한국어", 'KO test'!A26, IF($B$1="中文", 'ZH test'!A26, 'JP test'!A32))</f>
-        <v>禽冠状病毒的介电松弛效应及灭活。  </v>
+        <v>禽冠状病毒的介电松弛效应及灭活。</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF($B$1="한국어", 'KO test'!A27, IF($B$1="中文", 'ZH test'!A27, 'JP test'!A33))</f>
-        <v>冠状病毒基因组发明专利保护的思考。  </v>
+        <v>冠状病毒基因组发明专利保护的思考。</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF($B$1="한국어", 'KO test'!A28, IF($B$1="中文", 'ZH test'!A28, 'JP test'!A34))</f>
-        <v>中和试验进一步证明该分离病毒是一种犬冠状病毒。  </v>
+        <v>中和试验进一步证明该分离病毒是一种犬冠状病毒。</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF($B$1="한국어", 'KO test'!A29, IF($B$1="中文", 'ZH test'!A29, 'JP test'!A35))</f>
-        <v>基于密码子使用模式的冠状病毒亲缘关系分析。  </v>
+        <v>基于密码子使用模式的冠状病毒亲缘关系分析。</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF($B$1="한국어", 'KO test'!A30, IF($B$1="中文", 'ZH test'!A30, 'JP test'!A36))</f>
-        <v>猪呼吸道冠状病毒及实验室诊断方法研究进展。  </v>
+        <v>猪呼吸道冠状病毒及实验室诊断方法研究进展。</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF($B$1="한국어", 'KO test'!A31, IF($B$1="中文", 'ZH test'!A31, 'JP test'!A37))</f>
-        <v>与犬细小病毒，但没有具体的治疗犬冠状病毒。  </v>
+        <v>与犬细小病毒，但没有具体的治疗犬冠状病毒。</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF($B$1="한국어", 'KO test'!A32, IF($B$1="中文", 'ZH test'!A32, 'JP test'!A38))</f>
-        <v>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。  </v>
+        <v>突起蛋白是冠状病毒的主要抗原，包含许多抗原决定簇。</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF($B$1="한국어", 'KO test'!A33, IF($B$1="中文", 'ZH test'!A33, 'JP test'!A39))</f>
-        <v>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。 </v>
+        <v>从健康狐狸、貉粪中检出犬冠状病毒的两种基因型。</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF($B$1="한국어", 'KO test'!A34, IF($B$1="中文", 'ZH test'!A34, 'JP test'!A40))</f>
-        <v>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。  </v>
+        <v>大熊猫犬冠状病毒部分纤突蛋白基因的扩增与序列分析。</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF($B$1="한국어", 'KO test'!A35, IF($B$1="中文", 'ZH test'!A35, 'JP test'!A41))</f>
-        <v>病毒被反病毒软件删除了。  </v>
+        <v>病毒被反病毒软件删除了。</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF($B$1="한국어", 'KO test'!A36, IF($B$1="中文", 'ZH test'!A36, 'JP test'!A42))</f>
-        <v>他染上了一种致命病毒。  </v>
+        <v>他染上了一种致命病毒。</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF($B$1="한국어", 'KO test'!A37, IF($B$1="中文", 'ZH test'!A37, 'JP test'!A43))</f>
-        <v>血液检验显示有病毒存在。  </v>
+        <v>血液检验显示有病毒存在。</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF($B$1="한국어", 'KO test'!A38, IF($B$1="中文", 'ZH test'!A38, 'JP test'!A44))</f>
-        <v>哎呀，电脑又有病毒了。  </v>
+        <v>哎呀，电脑又有病毒了。</v>
       </c>
     </row>
   </sheetData>
@@ -842,102 +840,102 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -957,187 +955,187 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1149,200 +1147,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D58F233-F40F-4825-BB23-37CF2E70714B}">
   <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>